<commit_message>
Exp and roles added
</commit_message>
<xml_diff>
--- a/PMP/Exp.xlsx
+++ b/PMP/Exp.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="190">
   <si>
     <t>Skywire</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>Beverage Container Recycling</t>
-  </si>
-  <si>
-    <t>Airsweb</t>
   </si>
   <si>
     <t>Intenix</t>
@@ -1012,11 +1009,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE30"/>
+  <dimension ref="A1:AE29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1045,7 +1042,7 @@
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="P1" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q1" s="18"/>
       <c r="R1" s="18"/>
@@ -1061,90 +1058,166 @@
     </row>
     <row r="2" spans="1:31" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="E2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="P2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" s="5" t="s">
+      <c r="Q2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="V2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="W2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="X2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE2" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q2" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="R2" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="S2" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="T2" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="U2" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="V2" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="W2" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="X2" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y2" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z2" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="AD2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="AE2" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="12" t="s">
         <v>0</v>
+      </c>
+      <c r="C3" s="13">
+        <v>41639</v>
+      </c>
+      <c r="D3" s="13">
+        <v>41883</v>
+      </c>
+      <c r="E3" s="14">
+        <v>206</v>
+      </c>
+      <c r="F3" s="14">
+        <f>E3*9.5</f>
+        <v>1957</v>
+      </c>
+      <c r="G3" s="14">
+        <v>8</v>
+      </c>
+      <c r="H3" s="14">
+        <v>12</v>
+      </c>
+      <c r="I3" s="14">
+        <v>46</v>
+      </c>
+      <c r="J3" s="14">
+        <v>12</v>
+      </c>
+      <c r="K3" s="14">
+        <v>179</v>
+      </c>
+      <c r="L3" s="14">
+        <v>8</v>
+      </c>
+      <c r="M3" s="16">
+        <f>SUM(H3:L3)</f>
+        <v>257</v>
+      </c>
+      <c r="N3" s="14">
+        <v>6</v>
+      </c>
+      <c r="P3">
+        <f>31-5</f>
+        <v>26</v>
+      </c>
+      <c r="Q3">
+        <f>28-4</f>
+        <v>24</v>
+      </c>
+      <c r="R3">
+        <f>31-6</f>
+        <v>25</v>
+      </c>
+      <c r="S3">
+        <f>30-4</f>
+        <v>26</v>
+      </c>
+      <c r="T3">
+        <f>31-5</f>
+        <v>26</v>
+      </c>
+      <c r="U3">
+        <f>30-5</f>
+        <v>25</v>
+      </c>
+      <c r="V3">
+        <f>31-4</f>
+        <v>27</v>
+      </c>
+      <c r="W3">
+        <f>31-6</f>
+        <v>25</v>
+      </c>
+      <c r="X3">
+        <v>1</v>
+      </c>
+      <c r="AA3">
+        <v>1</v>
       </c>
       <c r="AD3" s="8">
         <v>300</v>
@@ -1268,22 +1341,23 @@
         <v>5</v>
       </c>
       <c r="H5" s="14">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="I5" s="14">
         <v>22</v>
       </c>
       <c r="J5" s="14">
-        <v>600</v>
+        <v>710</v>
       </c>
       <c r="K5" s="14">
         <v>4</v>
       </c>
       <c r="L5" s="14">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="M5" s="14">
-        <v>634</v>
+        <f>SUM(H5:L5)</f>
+        <v>758</v>
       </c>
       <c r="N5" s="14">
         <v>5</v>
@@ -1427,10 +1501,10 @@
         <v>3</v>
       </c>
       <c r="H7" s="14">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I7" s="14">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J7" s="14">
         <v>568</v>
@@ -1441,8 +1515,9 @@
       <c r="L7" s="14">
         <v>8</v>
       </c>
-      <c r="M7" s="14">
-        <v>632</v>
+      <c r="M7" s="16">
+        <f>SUM(H7:L7)</f>
+        <v>636</v>
       </c>
       <c r="N7" s="14">
         <v>2</v>
@@ -1474,14 +1549,76 @@
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="12" t="s">
         <v>5</v>
       </c>
+      <c r="C8" s="13">
+        <v>39829</v>
+      </c>
+      <c r="D8" s="13">
+        <v>40024</v>
+      </c>
+      <c r="E8" s="14">
+        <v>167</v>
+      </c>
+      <c r="F8" s="14">
+        <f>E8*8</f>
+        <v>1336</v>
+      </c>
+      <c r="G8" s="14">
+        <v>7</v>
+      </c>
+      <c r="H8" s="14">
+        <v>4</v>
+      </c>
+      <c r="I8" s="14">
+        <v>40</v>
+      </c>
+      <c r="J8" s="14">
+        <v>1039</v>
+      </c>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="16">
+        <f>SUM(H8:L8)</f>
+        <v>1083</v>
+      </c>
+      <c r="N8" s="14">
+        <v>7</v>
+      </c>
+      <c r="P8">
+        <f>16-3</f>
+        <v>13</v>
+      </c>
+      <c r="Q8">
+        <f>28-4</f>
+        <v>24</v>
+      </c>
+      <c r="R8">
+        <f>31-6</f>
+        <v>25</v>
+      </c>
+      <c r="S8">
+        <f>30-4</f>
+        <v>26</v>
+      </c>
+      <c r="T8">
+        <f>31-5</f>
+        <v>26</v>
+      </c>
+      <c r="U8">
+        <f>30-4</f>
+        <v>26</v>
+      </c>
+      <c r="V8">
+        <f>31-4</f>
+        <v>27</v>
+      </c>
       <c r="AD8" s="8">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="AE8" s="8">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
@@ -1492,72 +1629,76 @@
         <v>6</v>
       </c>
       <c r="C9" s="13">
-        <v>39829</v>
+        <v>40779</v>
       </c>
       <c r="D9" s="13">
-        <v>40024</v>
-      </c>
-      <c r="E9" s="14">
-        <v>167</v>
+        <v>40952</v>
+      </c>
+      <c r="E9" s="16">
+        <v>142</v>
       </c>
       <c r="F9" s="14">
         <f>E9*8</f>
-        <v>1336</v>
-      </c>
-      <c r="G9" s="14">
-        <v>7</v>
-      </c>
-      <c r="H9" s="14">
-        <v>4</v>
-      </c>
-      <c r="I9" s="14">
-        <v>40</v>
-      </c>
-      <c r="J9" s="14">
-        <v>1260</v>
-      </c>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
+        <v>1136</v>
+      </c>
+      <c r="G9" s="16">
+        <v>6</v>
+      </c>
+      <c r="H9" s="16">
+        <v>0</v>
+      </c>
+      <c r="I9" s="16">
+        <v>156</v>
+      </c>
+      <c r="J9" s="16">
+        <v>793</v>
+      </c>
+      <c r="K9" s="16">
+        <v>16</v>
+      </c>
+      <c r="L9" s="16">
+        <v>24</v>
+      </c>
       <c r="M9" s="16">
         <f>SUM(H9:L9)</f>
-        <v>1304</v>
-      </c>
-      <c r="N9" s="14">
-        <v>7</v>
+        <v>989</v>
+      </c>
+      <c r="N9" s="17">
+        <v>6</v>
       </c>
       <c r="P9">
-        <f>16-3</f>
-        <v>13</v>
-      </c>
-      <c r="Q9">
-        <f>28-4</f>
-        <v>24</v>
-      </c>
-      <c r="R9">
         <f>31-6</f>
         <v>25</v>
       </c>
-      <c r="S9">
-        <f>30-4</f>
-        <v>26</v>
-      </c>
-      <c r="T9">
-        <f>31-5</f>
-        <v>26</v>
-      </c>
-      <c r="U9">
-        <f>30-4</f>
-        <v>26</v>
-      </c>
-      <c r="V9">
+      <c r="Q9">
+        <f>12-2</f>
+        <v>10</v>
+      </c>
+      <c r="W9">
+        <v>7</v>
+      </c>
+      <c r="X9">
+        <f>30-5</f>
+        <v>25</v>
+      </c>
+      <c r="Y9">
+        <f>31-6</f>
+        <v>25</v>
+      </c>
+      <c r="Z9">
+        <f>30-7</f>
+        <v>23</v>
+      </c>
+      <c r="AA9">
         <f>31-4</f>
         <v>27</v>
       </c>
-      <c r="AD9" s="8">
-        <v>500</v>
-      </c>
-      <c r="AE9" s="8">
-        <v>6</v>
+      <c r="AD9" s="4">
+        <f>SUM(Y9:AC9)</f>
+        <v>75</v>
+      </c>
+      <c r="AE9" s="1">
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
@@ -1565,143 +1706,70 @@
         <v>8</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C10" s="13">
-        <v>40779</v>
+        <v>42804</v>
       </c>
       <c r="D10" s="13">
-        <v>40952</v>
-      </c>
-      <c r="E10" s="16">
-        <v>142</v>
-      </c>
-      <c r="F10" s="14"/>
-      <c r="G10" s="16">
+        <v>42975</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="14">
+        <v>172.5</v>
+      </c>
+      <c r="G10" s="14">
         <v>6</v>
       </c>
-      <c r="H10" s="16">
-        <v>0</v>
-      </c>
-      <c r="I10" s="16">
-        <v>156</v>
-      </c>
-      <c r="J10" s="16">
-        <v>940</v>
-      </c>
-      <c r="K10" s="16">
-        <v>16</v>
-      </c>
-      <c r="L10" s="16">
-        <v>24</v>
-      </c>
+      <c r="H10" s="14">
+        <v>12</v>
+      </c>
+      <c r="I10" s="14">
+        <v>23</v>
+      </c>
+      <c r="J10" s="14">
+        <v>16.5</v>
+      </c>
+      <c r="K10" s="14">
+        <v>129</v>
+      </c>
+      <c r="L10" s="14"/>
       <c r="M10" s="16">
         <f>SUM(H10:L10)</f>
-        <v>1136</v>
-      </c>
-      <c r="N10" s="17">
-        <v>6</v>
-      </c>
-      <c r="P10">
-        <f>31-6</f>
-        <v>25</v>
-      </c>
-      <c r="Q10">
-        <f>12-2</f>
-        <v>10</v>
+        <v>180.5</v>
+      </c>
+      <c r="N10" s="14"/>
+      <c r="R10">
+        <v>24</v>
+      </c>
+      <c r="S10">
+        <v>23</v>
+      </c>
+      <c r="T10">
+        <v>23</v>
+      </c>
+      <c r="U10">
+        <v>35</v>
+      </c>
+      <c r="V10">
+        <v>35</v>
       </c>
       <c r="W10">
-        <v>7</v>
-      </c>
-      <c r="X10">
-        <f>30-5</f>
-        <v>25</v>
-      </c>
-      <c r="Y10">
-        <f>31-6</f>
-        <v>25</v>
-      </c>
-      <c r="Z10">
-        <f>30-7</f>
-        <v>23</v>
-      </c>
-      <c r="AA10">
-        <f>31-4</f>
-        <v>27</v>
+        <v>32.5</v>
       </c>
       <c r="AD10" s="4">
         <f>SUM(Y10:AC10)</f>
-        <v>75</v>
-      </c>
-      <c r="AE10" s="1">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="AE10" s="8">
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="13">
-        <v>42804</v>
-      </c>
-      <c r="D11" s="13">
-        <v>42975</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" s="14">
-        <v>172.5</v>
-      </c>
-      <c r="G11" s="14">
-        <v>6</v>
-      </c>
-      <c r="H11" s="14">
-        <v>12</v>
-      </c>
-      <c r="I11" s="14">
-        <v>23</v>
-      </c>
-      <c r="J11" s="14">
-        <v>16.5</v>
-      </c>
-      <c r="K11" s="14">
-        <v>129</v>
-      </c>
-      <c r="L11" s="14"/>
-      <c r="M11" s="16">
-        <f>SUM(H11:L11)</f>
-        <v>180.5</v>
-      </c>
-      <c r="N11" s="14"/>
-      <c r="R11">
-        <v>24</v>
-      </c>
-      <c r="S11">
-        <v>23</v>
-      </c>
-      <c r="T11">
-        <v>23</v>
-      </c>
-      <c r="U11">
-        <v>35</v>
-      </c>
-      <c r="V11">
-        <v>35</v>
-      </c>
-      <c r="W11">
-        <v>32.5</v>
-      </c>
-      <c r="AD11" s="4">
-        <f>SUM(Y11:AC11)</f>
-        <v>0</v>
-      </c>
-      <c r="AE11" s="8">
-        <v>6</v>
-      </c>
+      <c r="AD11" s="8"/>
+      <c r="AE11" s="8"/>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="AD12" s="8"/>
@@ -1712,164 +1780,174 @@
       <c r="AE13" s="8"/>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="AD14" s="8"/>
-      <c r="AE14" s="8"/>
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD14" s="8">
+        <v>150</v>
+      </c>
+      <c r="AE14" s="8">
+        <v>8</v>
+      </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
       </c>
+      <c r="C15" s="3">
+        <v>42622</v>
+      </c>
+      <c r="D15" s="3">
+        <v>42776</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="2">
+        <v>42</v>
+      </c>
+      <c r="H15" s="2">
+        <v>3</v>
+      </c>
+      <c r="I15" s="2">
+        <v>13</v>
+      </c>
+      <c r="K15" s="2">
+        <v>22</v>
+      </c>
+      <c r="L15" s="2">
+        <v>4</v>
+      </c>
+      <c r="P15">
+        <v>12</v>
+      </c>
+      <c r="Q15">
+        <v>3</v>
+      </c>
+      <c r="X15">
+        <v>43</v>
+      </c>
+      <c r="Y15">
+        <v>5</v>
+      </c>
+      <c r="Z15">
+        <v>7</v>
+      </c>
+      <c r="AA15">
+        <v>9</v>
+      </c>
       <c r="AD15" s="8">
-        <v>150</v>
+        <v>175</v>
       </c>
       <c r="AE15" s="8">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B16" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="3">
-        <v>42622</v>
-      </c>
-      <c r="D16" s="3">
-        <v>42776</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" s="2">
-        <v>42</v>
-      </c>
-      <c r="H16" s="2">
-        <v>3</v>
-      </c>
-      <c r="I16" s="2">
-        <v>13</v>
-      </c>
-      <c r="K16" s="2">
-        <v>22</v>
-      </c>
-      <c r="L16" s="2">
-        <v>4</v>
-      </c>
-      <c r="P16">
-        <v>12</v>
-      </c>
-      <c r="Q16">
-        <v>3</v>
-      </c>
-      <c r="X16">
-        <v>43</v>
-      </c>
-      <c r="Y16">
-        <v>5</v>
-      </c>
-      <c r="Z16">
-        <v>7</v>
-      </c>
-      <c r="AA16">
-        <v>9</v>
-      </c>
       <c r="AD16" s="8">
-        <v>175</v>
+        <v>60</v>
       </c>
       <c r="AE16" s="8">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
       </c>
       <c r="AD17" s="8">
-        <v>60</v>
+        <v>250</v>
       </c>
       <c r="AE17" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
         <v>11</v>
       </c>
+      <c r="C18" s="3">
+        <v>42853</v>
+      </c>
+      <c r="D18" s="3">
+        <v>42976</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="2">
+        <v>91</v>
+      </c>
+      <c r="G18" s="2">
+        <v>4</v>
+      </c>
+      <c r="H18" s="2">
+        <v>14</v>
+      </c>
+      <c r="I18" s="2">
+        <v>32</v>
+      </c>
+      <c r="J18" s="2">
+        <v>2</v>
+      </c>
+      <c r="K18" s="2">
+        <v>39</v>
+      </c>
+      <c r="L18" s="2">
+        <v>4</v>
+      </c>
+      <c r="N18" s="2">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>24</v>
+      </c>
+      <c r="T18">
+        <v>23</v>
+      </c>
+      <c r="U18">
+        <v>10</v>
+      </c>
+      <c r="V18">
+        <v>10</v>
+      </c>
+      <c r="W18">
+        <v>24</v>
+      </c>
       <c r="AD18" s="8">
-        <v>250</v>
+        <v>75</v>
       </c>
       <c r="AE18" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B19" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="3">
-        <v>42853</v>
-      </c>
-      <c r="D19" s="3">
-        <v>42976</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F19" s="2">
-        <v>91</v>
-      </c>
-      <c r="G19" s="2">
-        <v>4</v>
-      </c>
-      <c r="H19" s="2">
-        <v>14</v>
-      </c>
-      <c r="I19" s="2">
-        <v>32</v>
-      </c>
-      <c r="J19" s="2">
-        <v>2</v>
-      </c>
-      <c r="K19" s="2">
-        <v>39</v>
-      </c>
-      <c r="L19" s="2">
-        <v>4</v>
-      </c>
-      <c r="N19" s="2">
-        <v>0</v>
-      </c>
-      <c r="S19">
-        <v>24</v>
-      </c>
-      <c r="T19">
-        <v>23</v>
-      </c>
-      <c r="U19">
-        <v>10</v>
-      </c>
-      <c r="V19">
-        <v>10</v>
-      </c>
-      <c r="W19">
-        <v>24</v>
-      </c>
       <c r="AD19" s="8">
-        <v>75</v>
+        <v>125</v>
       </c>
       <c r="AE19" s="8">
         <v>4</v>
@@ -1877,263 +1955,249 @@
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B20" t="s">
         <v>13</v>
       </c>
       <c r="AD20" s="8">
-        <v>125</v>
+        <v>60</v>
       </c>
       <c r="AE20" s="8">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>16</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="AD21" s="8"/>
+      <c r="AE21" s="8"/>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s">
         <v>14</v>
       </c>
-      <c r="AD21" s="8">
-        <v>60</v>
-      </c>
-      <c r="AE21" s="8">
+      <c r="C22" s="3">
+        <v>42697</v>
+      </c>
+      <c r="D22" s="3">
+        <v>42752</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="2">
+        <v>42</v>
+      </c>
+      <c r="G22" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="AD22" s="8"/>
-      <c r="AE22" s="8"/>
+      <c r="H22" s="2">
+        <v>2</v>
+      </c>
+      <c r="I22" s="2">
+        <v>14</v>
+      </c>
+      <c r="J22" s="2">
+        <v>5</v>
+      </c>
+      <c r="K22" s="2">
+        <v>19</v>
+      </c>
+      <c r="L22" s="2">
+        <v>2</v>
+      </c>
+      <c r="P22">
+        <v>19</v>
+      </c>
+      <c r="Q22">
+        <v>21</v>
+      </c>
+      <c r="Z22">
+        <v>1.5</v>
+      </c>
+      <c r="AA22">
+        <v>13</v>
+      </c>
+      <c r="AD22" s="8">
+        <v>100</v>
+      </c>
+      <c r="AE22" s="8">
+        <v>3</v>
+      </c>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B23" t="s">
         <v>15</v>
       </c>
       <c r="C23" s="3">
-        <v>42697</v>
+        <v>42817</v>
       </c>
       <c r="D23" s="3">
-        <v>42752</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>42</v>
+        <v>42879</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>41</v>
       </c>
       <c r="F23" s="2">
-        <v>42</v>
+        <v>109</v>
       </c>
       <c r="G23" s="2">
         <v>2</v>
       </c>
       <c r="H23" s="2">
+        <v>4</v>
+      </c>
+      <c r="I23" s="2">
+        <v>28</v>
+      </c>
+      <c r="K23" s="2">
+        <v>69</v>
+      </c>
+      <c r="L23" s="2">
+        <v>8</v>
+      </c>
+      <c r="N23" s="2">
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <v>16</v>
+      </c>
+      <c r="S23">
+        <v>51</v>
+      </c>
+      <c r="T23">
+        <v>42</v>
+      </c>
+      <c r="AD23" s="8">
+        <v>80</v>
+      </c>
+      <c r="AE23" s="8">
         <v>2</v>
-      </c>
-      <c r="I23" s="2">
-        <v>14</v>
-      </c>
-      <c r="J23" s="2">
-        <v>5</v>
-      </c>
-      <c r="K23" s="2">
-        <v>19</v>
-      </c>
-      <c r="L23" s="2">
-        <v>2</v>
-      </c>
-      <c r="P23">
-        <v>19</v>
-      </c>
-      <c r="Q23">
-        <v>21</v>
-      </c>
-      <c r="Z23">
-        <v>1.5</v>
-      </c>
-      <c r="AA23">
-        <v>13</v>
-      </c>
-      <c r="AD23" s="8">
-        <v>100</v>
-      </c>
-      <c r="AE23" s="8">
-        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B24" t="s">
         <v>16</v>
       </c>
       <c r="C24" s="3">
-        <v>42817</v>
+        <v>42690</v>
       </c>
       <c r="D24" s="3">
-        <v>42879</v>
+        <v>42832</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F24" s="2">
-        <v>109</v>
+        <v>134</v>
       </c>
       <c r="G24" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H24" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I24" s="2">
-        <v>28</v>
+        <v>38</v>
+      </c>
+      <c r="J24" s="2">
+        <v>6</v>
       </c>
       <c r="K24" s="2">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="L24" s="2">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="N24" s="2">
         <v>0</v>
       </c>
+      <c r="P24">
+        <v>16</v>
+      </c>
+      <c r="Q24">
+        <v>23</v>
+      </c>
       <c r="R24">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="S24">
-        <v>51</v>
-      </c>
-      <c r="T24">
+        <v>22</v>
+      </c>
+      <c r="Z24">
+        <v>22</v>
+      </c>
+      <c r="AA24">
+        <v>20</v>
+      </c>
+      <c r="AD24" s="8">
+        <v>200</v>
+      </c>
+      <c r="AE24" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AD25" s="8"/>
+      <c r="AE25" s="8"/>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="L26" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="AD24" s="8">
-        <v>80</v>
-      </c>
-      <c r="AE24" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>19</v>
-      </c>
-      <c r="B25" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" s="3">
-        <v>42690</v>
-      </c>
-      <c r="D25" s="3">
-        <v>42832</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F25" s="2">
-        <v>134</v>
-      </c>
-      <c r="G25" s="2">
-        <v>5</v>
-      </c>
-      <c r="H25" s="2">
-        <v>6</v>
-      </c>
-      <c r="I25" s="2">
-        <v>38</v>
-      </c>
-      <c r="J25" s="2">
-        <v>6</v>
-      </c>
-      <c r="K25" s="2">
-        <v>74</v>
-      </c>
-      <c r="L25" s="2">
-        <v>10</v>
-      </c>
-      <c r="N25" s="2">
-        <v>0</v>
-      </c>
-      <c r="P25">
-        <v>16</v>
-      </c>
-      <c r="Q25">
-        <v>23</v>
-      </c>
-      <c r="R25">
-        <v>31</v>
-      </c>
-      <c r="S25">
-        <v>22</v>
-      </c>
-      <c r="Z25">
-        <v>22</v>
-      </c>
-      <c r="AA25">
-        <v>20</v>
-      </c>
-      <c r="AD25" s="8">
-        <v>200</v>
-      </c>
-      <c r="AE25" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="AD26" s="8"/>
-      <c r="AE26" s="8"/>
+      <c r="M26" s="5">
+        <f>SUM(M3:M24)</f>
+        <v>4520.5</v>
+      </c>
+      <c r="N26" s="5">
+        <f>SUM(N3:N24)</f>
+        <v>43</v>
+      </c>
+      <c r="AD26" s="5">
+        <f>SUM(AD3:AD24)</f>
+        <v>3750</v>
+      </c>
+      <c r="AE26" s="5">
+        <f>SUM(AE3:AE24)</f>
+        <v>87</v>
+      </c>
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="L27" s="5" t="s">
+      <c r="AD27" s="8"/>
+      <c r="AE27" s="8"/>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="L28" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="M27" s="5">
-        <f>SUM(M3:M25)</f>
-        <v>4503.5</v>
-      </c>
-      <c r="N27" s="5">
-        <f>SUM(N3:N25)</f>
-        <v>37</v>
-      </c>
-      <c r="AD27" s="5">
-        <f>SUM(AD3:AD25)</f>
-        <v>3850</v>
-      </c>
-      <c r="AE27" s="5">
-        <f>SUM(AE3:AE25)</f>
-        <v>89</v>
-      </c>
-    </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="AD28" s="8"/>
-      <c r="AE28" s="8"/>
+      <c r="M28" s="6">
+        <f>4500-M26</f>
+        <v>-20.5</v>
+      </c>
+      <c r="N28" s="6">
+        <f>36-N26</f>
+        <v>-7</v>
+      </c>
+      <c r="AD28" s="6">
+        <f>4500-AD26</f>
+        <v>750</v>
+      </c>
+      <c r="AE28" s="6">
+        <f>36-AE26</f>
+        <v>-51</v>
+      </c>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="L29" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="M29" s="6">
-        <f>4500-M27</f>
-        <v>-3.5</v>
-      </c>
-      <c r="N29" s="6">
-        <f>36-N27</f>
-        <v>-1</v>
-      </c>
-      <c r="AD29" s="6">
-        <f>4500-AD27</f>
-        <v>650</v>
-      </c>
-      <c r="AE29" s="6">
-        <f>36-AE27</f>
-        <v>-53</v>
-      </c>
-    </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="AD30" s="8"/>
-      <c r="AE30" s="8"/>
+      <c r="AD29" s="8"/>
+      <c r="AE29" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2142,7 +2206,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="M10" formulaRange="1"/>
+    <ignoredError sqref="M9" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -2159,52 +2223,52 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
         <v>50</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>51</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
         <v>52</v>
       </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>53</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>54</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>55</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>56</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>57</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>58</v>
-      </c>
-      <c r="K5" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -2212,44 +2276,44 @@
         <v>42977</v>
       </c>
       <c r="B6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" t="s">
         <v>60</v>
-      </c>
-      <c r="C6" t="s">
-        <v>61</v>
       </c>
       <c r="D6" s="10">
         <v>6.25E-2</v>
       </c>
       <c r="E6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" t="s">
         <v>62</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>63</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>64</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>65</v>
-      </c>
-      <c r="I6" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" t="s">
         <v>68</v>
       </c>
-      <c r="B8" t="s">
-        <v>69</v>
-      </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -2257,64 +2321,64 @@
         <v>42977</v>
       </c>
       <c r="B9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" t="s">
         <v>60</v>
-      </c>
-      <c r="C9" t="s">
-        <v>61</v>
       </c>
       <c r="D9" s="10">
         <v>0.33333333333333331</v>
       </c>
       <c r="E9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" t="s">
         <v>62</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>63</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>64</v>
       </c>
-      <c r="H9" t="s">
-        <v>65</v>
-      </c>
       <c r="I9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -2322,39 +2386,39 @@
         <v>42976</v>
       </c>
       <c r="B16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" t="s">
         <v>60</v>
-      </c>
-      <c r="C16" t="s">
-        <v>61</v>
       </c>
       <c r="D16" s="10">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="E16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16" t="s">
         <v>62</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>63</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>64</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>65</v>
-      </c>
-      <c r="I16" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -2362,54 +2426,54 @@
         <v>42976</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D18" s="10">
         <v>0.375</v>
       </c>
       <c r="E18" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" t="s">
+        <v>62</v>
+      </c>
+      <c r="G18" t="s">
+        <v>63</v>
+      </c>
+      <c r="H18" t="s">
+        <v>64</v>
+      </c>
+      <c r="I18" t="s">
         <v>79</v>
-      </c>
-      <c r="F18" t="s">
-        <v>63</v>
-      </c>
-      <c r="G18" t="s">
-        <v>64</v>
-      </c>
-      <c r="H18" t="s">
-        <v>65</v>
-      </c>
-      <c r="I18" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -2417,39 +2481,39 @@
         <v>42972</v>
       </c>
       <c r="B23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" t="s">
         <v>60</v>
-      </c>
-      <c r="C23" t="s">
-        <v>61</v>
       </c>
       <c r="D23" s="10">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="E23" t="s">
+        <v>61</v>
+      </c>
+      <c r="F23" t="s">
         <v>62</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>63</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>64</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>65</v>
-      </c>
-      <c r="I23" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -2457,34 +2521,34 @@
         <v>42972</v>
       </c>
       <c r="B25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D25" s="10">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="E25" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" t="s">
         <v>62</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>63</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>64</v>
       </c>
-      <c r="H25" t="s">
-        <v>65</v>
-      </c>
       <c r="I25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -2492,39 +2556,39 @@
         <v>42971</v>
       </c>
       <c r="B26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D26" s="10">
         <v>1.2499999999999999E-2</v>
       </c>
       <c r="E26" t="s">
+        <v>61</v>
+      </c>
+      <c r="F26" t="s">
         <v>62</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>63</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>64</v>
       </c>
-      <c r="H26" t="s">
-        <v>65</v>
-      </c>
       <c r="I26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -2532,44 +2596,44 @@
         <v>42971</v>
       </c>
       <c r="B28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D28" s="10">
         <v>0.38750000000000001</v>
       </c>
       <c r="E28" t="s">
+        <v>61</v>
+      </c>
+      <c r="F28" t="s">
         <v>62</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>63</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>64</v>
       </c>
-      <c r="H28" t="s">
-        <v>65</v>
-      </c>
       <c r="I28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -2577,49 +2641,49 @@
         <v>42970</v>
       </c>
       <c r="B31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D31" s="10">
         <v>0.17916666666666667</v>
       </c>
       <c r="E31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F31" t="s">
+        <v>62</v>
+      </c>
+      <c r="G31" t="s">
         <v>63</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>64</v>
       </c>
-      <c r="H31" t="s">
+      <c r="I31" t="s">
         <v>65</v>
-      </c>
-      <c r="I31" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C34" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -2627,54 +2691,54 @@
         <v>42970</v>
       </c>
       <c r="B35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C35" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D35" s="10">
         <v>0.22083333333333333</v>
       </c>
       <c r="E35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F35" t="s">
+        <v>62</v>
+      </c>
+      <c r="G35" t="s">
         <v>63</v>
       </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
         <v>64</v>
       </c>
-      <c r="H35" t="s">
-        <v>65</v>
-      </c>
       <c r="I35" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C39" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -2682,44 +2746,44 @@
         <v>42969</v>
       </c>
       <c r="B40" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C40" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D40" s="10">
         <v>5.4166666666666669E-2</v>
       </c>
       <c r="E40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F40" t="s">
+        <v>62</v>
+      </c>
+      <c r="G40" t="s">
         <v>63</v>
       </c>
-      <c r="G40" t="s">
+      <c r="H40" t="s">
         <v>64</v>
       </c>
-      <c r="H40" t="s">
+      <c r="I40" t="s">
         <v>65</v>
-      </c>
-      <c r="I40" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C42" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -2727,54 +2791,54 @@
         <v>42969</v>
       </c>
       <c r="B43" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C43" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D43" s="10">
         <v>0.34583333333333338</v>
       </c>
       <c r="E43" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F43" t="s">
+        <v>62</v>
+      </c>
+      <c r="G43" t="s">
         <v>63</v>
       </c>
-      <c r="G43" t="s">
+      <c r="H43" t="s">
         <v>64</v>
       </c>
-      <c r="H43" t="s">
-        <v>65</v>
-      </c>
       <c r="I43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B47" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C47" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -2782,44 +2846,44 @@
         <v>42968</v>
       </c>
       <c r="B48" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C48" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D48" s="10">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E48" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F48" t="s">
+        <v>62</v>
+      </c>
+      <c r="G48" t="s">
         <v>63</v>
       </c>
-      <c r="G48" t="s">
+      <c r="H48" t="s">
         <v>64</v>
       </c>
-      <c r="H48" t="s">
+      <c r="I48" t="s">
         <v>65</v>
-      </c>
-      <c r="I48" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B50" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C50" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -2827,34 +2891,34 @@
         <v>42968</v>
       </c>
       <c r="B51" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C51" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D51" s="10">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E51" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F51" t="s">
+        <v>62</v>
+      </c>
+      <c r="G51" t="s">
         <v>63</v>
       </c>
-      <c r="G51" t="s">
+      <c r="H51" t="s">
         <v>64</v>
       </c>
-      <c r="H51" t="s">
-        <v>65</v>
-      </c>
       <c r="I51" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J51" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K51" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -2862,39 +2926,39 @@
         <v>42968</v>
       </c>
       <c r="B52" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C52" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D52" s="10">
         <v>5.4166666666666669E-2</v>
       </c>
       <c r="E52" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F52" t="s">
+        <v>62</v>
+      </c>
+      <c r="G52" t="s">
         <v>63</v>
       </c>
-      <c r="G52" t="s">
+      <c r="H52" t="s">
         <v>64</v>
       </c>
-      <c r="H52" t="s">
-        <v>65</v>
-      </c>
       <c r="I52" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B53" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C53" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -2902,44 +2966,44 @@
         <v>42968</v>
       </c>
       <c r="B54" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C54" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D54" s="10">
         <v>0.20833333333333334</v>
       </c>
       <c r="E54" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F54" t="s">
+        <v>62</v>
+      </c>
+      <c r="G54" t="s">
         <v>63</v>
       </c>
-      <c r="G54" t="s">
+      <c r="H54" t="s">
         <v>64</v>
       </c>
-      <c r="H54" t="s">
-        <v>65</v>
-      </c>
       <c r="I54" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B56" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C56" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
@@ -2947,69 +3011,69 @@
         <v>42965</v>
       </c>
       <c r="B57" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C57" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D57" s="10">
         <v>0.39583333333333331</v>
       </c>
       <c r="E57" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F57" t="s">
+        <v>62</v>
+      </c>
+      <c r="G57" t="s">
         <v>63</v>
       </c>
-      <c r="G57" t="s">
+      <c r="H57" t="s">
         <v>64</v>
       </c>
-      <c r="H57" t="s">
-        <v>65</v>
-      </c>
       <c r="I57" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B64" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C64" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -3017,54 +3081,54 @@
         <v>42964</v>
       </c>
       <c r="B65" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C65" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D65" s="10">
         <v>0.39583333333333331</v>
       </c>
       <c r="E65" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F65" t="s">
+        <v>62</v>
+      </c>
+      <c r="G65" t="s">
         <v>63</v>
       </c>
-      <c r="G65" t="s">
+      <c r="H65" t="s">
         <v>64</v>
       </c>
-      <c r="H65" t="s">
-        <v>65</v>
-      </c>
       <c r="I65" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B69" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C69" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -3072,64 +3136,64 @@
         <v>42963</v>
       </c>
       <c r="B70" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C70" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D70" s="10">
         <v>0.39583333333333331</v>
       </c>
       <c r="E70" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F70" t="s">
+        <v>62</v>
+      </c>
+      <c r="G70" t="s">
         <v>63</v>
       </c>
-      <c r="G70" t="s">
+      <c r="H70" t="s">
         <v>64</v>
       </c>
-      <c r="H70" t="s">
-        <v>65</v>
-      </c>
       <c r="I70" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B76" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C76" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -3137,56 +3201,56 @@
         <v>42961</v>
       </c>
       <c r="B77" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C77" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D77" s="10">
         <v>0.39583333333333331</v>
       </c>
       <c r="E77" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F77" t="s">
+        <v>62</v>
+      </c>
+      <c r="G77" t="s">
         <v>63</v>
       </c>
-      <c r="G77" t="s">
+      <c r="H77" t="s">
         <v>64</v>
       </c>
-      <c r="H77" t="s">
+      <c r="I77" t="s">
         <v>65</v>
-      </c>
-      <c r="I77" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C82" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
@@ -3194,64 +3258,64 @@
         <v>42958</v>
       </c>
       <c r="B83" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C83" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D83" s="10">
         <v>0.39583333333333331</v>
       </c>
       <c r="E83" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F83" t="s">
+        <v>62</v>
+      </c>
+      <c r="G83" t="s">
         <v>63</v>
       </c>
-      <c r="G83" t="s">
+      <c r="H83" t="s">
         <v>64</v>
       </c>
-      <c r="H83" t="s">
+      <c r="I83" t="s">
         <v>65</v>
-      </c>
-      <c r="I83" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B89" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C89" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -3259,59 +3323,59 @@
         <v>42957</v>
       </c>
       <c r="B90" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C90" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D90" s="10">
         <v>0.39583333333333331</v>
       </c>
       <c r="E90" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F90" t="s">
+        <v>62</v>
+      </c>
+      <c r="G90" t="s">
         <v>63</v>
       </c>
-      <c r="G90" t="s">
+      <c r="H90" t="s">
         <v>64</v>
       </c>
-      <c r="H90" t="s">
+      <c r="I90" t="s">
         <v>65</v>
-      </c>
-      <c r="I90" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B95" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C95" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
@@ -3319,64 +3383,64 @@
         <v>42956</v>
       </c>
       <c r="B96" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C96" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D96" s="10">
         <v>0.39583333333333331</v>
       </c>
       <c r="E96" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F96" t="s">
+        <v>62</v>
+      </c>
+      <c r="G96" t="s">
         <v>63</v>
       </c>
-      <c r="G96" t="s">
+      <c r="H96" t="s">
         <v>64</v>
       </c>
-      <c r="H96" t="s">
+      <c r="I96" t="s">
         <v>65</v>
-      </c>
-      <c r="I96" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B102" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C102" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
@@ -3384,64 +3448,64 @@
         <v>42955</v>
       </c>
       <c r="B103" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C103" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D103" s="10">
         <v>0.39583333333333331</v>
       </c>
       <c r="E103" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F103" t="s">
+        <v>62</v>
+      </c>
+      <c r="G103" t="s">
         <v>63</v>
       </c>
-      <c r="G103" t="s">
+      <c r="H103" t="s">
         <v>64</v>
       </c>
-      <c r="H103" t="s">
-        <v>65</v>
-      </c>
       <c r="I103" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B109" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C109" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
@@ -3449,59 +3513,59 @@
         <v>42954</v>
       </c>
       <c r="B110" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C110" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D110" s="10">
         <v>0.39583333333333331</v>
       </c>
       <c r="E110" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F110" t="s">
+        <v>62</v>
+      </c>
+      <c r="G110" t="s">
         <v>63</v>
       </c>
-      <c r="G110" t="s">
+      <c r="H110" t="s">
         <v>64</v>
       </c>
-      <c r="H110" t="s">
+      <c r="I110" t="s">
         <v>65</v>
-      </c>
-      <c r="I110" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B115" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C115" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
@@ -3509,59 +3573,59 @@
         <v>42951</v>
       </c>
       <c r="B116" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C116" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D116" s="10">
         <v>0.39583333333333331</v>
       </c>
       <c r="E116" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F116" t="s">
+        <v>62</v>
+      </c>
+      <c r="G116" t="s">
         <v>63</v>
       </c>
-      <c r="G116" t="s">
+      <c r="H116" t="s">
         <v>64</v>
       </c>
-      <c r="H116" t="s">
+      <c r="I116" t="s">
         <v>65</v>
-      </c>
-      <c r="I116" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B121" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C121" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
@@ -3569,53 +3633,53 @@
         <v>42950</v>
       </c>
       <c r="B122" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C122" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D122" s="10">
         <v>0.4291666666666667</v>
       </c>
       <c r="E122" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F122" t="s">
+        <v>62</v>
+      </c>
+      <c r="G122" t="s">
         <v>63</v>
       </c>
-      <c r="G122" t="s">
+      <c r="H122" t="s">
         <v>64</v>
       </c>
-      <c r="H122" t="s">
-        <v>65</v>
-      </c>
       <c r="I122" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
@@ -3636,10 +3700,10 @@
         <v>#NAME?</v>
       </c>
       <c r="B130" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C130" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
@@ -3647,59 +3711,59 @@
         <v>42949</v>
       </c>
       <c r="B131" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C131" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D131" s="10">
         <v>0.39583333333333331</v>
       </c>
       <c r="E131" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F131" t="s">
+        <v>62</v>
+      </c>
+      <c r="G131" t="s">
         <v>63</v>
       </c>
-      <c r="G131" t="s">
+      <c r="H131" t="s">
         <v>64</v>
       </c>
-      <c r="H131" t="s">
-        <v>65</v>
-      </c>
       <c r="I131" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B136" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C136" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
@@ -3707,94 +3771,94 @@
         <v>42948</v>
       </c>
       <c r="B137" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C137" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D137" s="10">
         <v>0.39583333333333331</v>
       </c>
       <c r="E137" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F137" t="s">
+        <v>62</v>
+      </c>
+      <c r="G137" t="s">
         <v>63</v>
       </c>
-      <c r="G137" t="s">
+      <c r="H137" t="s">
         <v>64</v>
       </c>
-      <c r="H137" t="s">
+      <c r="I137" t="s">
         <v>65</v>
-      </c>
-      <c r="I137" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B142" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C142" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
+        <v>49</v>
+      </c>
+      <c r="B145" t="s">
         <v>50</v>
       </c>
-      <c r="B145" t="s">
-        <v>51</v>
-      </c>
       <c r="C145" t="s">
+        <v>176</v>
+      </c>
+      <c r="D145" t="s">
+        <v>21</v>
+      </c>
+      <c r="E145" t="s">
         <v>177</v>
       </c>
-      <c r="D145" t="s">
-        <v>22</v>
-      </c>
-      <c r="E145" t="s">
-        <v>178</v>
-      </c>
       <c r="F145" t="s">
+        <v>53</v>
+      </c>
+      <c r="G145" t="s">
         <v>54</v>
       </c>
-      <c r="G145" t="s">
+      <c r="H145" t="s">
         <v>55</v>
       </c>
-      <c r="H145" t="s">
+      <c r="I145" t="s">
         <v>56</v>
       </c>
-      <c r="I145" t="s">
+      <c r="J145" t="s">
         <v>57</v>
       </c>
-      <c r="J145" t="s">
+      <c r="K145" t="s">
         <v>58</v>
-      </c>
-      <c r="K145" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="146" spans="1:11" x14ac:dyDescent="0.25">
@@ -3802,34 +3866,34 @@
         <v>42975</v>
       </c>
       <c r="B146" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C146" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D146" s="10">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="E146" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F146" t="s">
+        <v>62</v>
+      </c>
+      <c r="G146" t="s">
         <v>63</v>
       </c>
-      <c r="G146" t="s">
+      <c r="H146" t="s">
         <v>64</v>
       </c>
-      <c r="H146" t="s">
-        <v>65</v>
-      </c>
       <c r="I146" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J146" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K146" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="147" spans="1:11" x14ac:dyDescent="0.25">
@@ -3837,54 +3901,54 @@
         <v>42975</v>
       </c>
       <c r="B147" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C147" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D147" s="10">
         <v>0.35416666666666669</v>
       </c>
       <c r="E147" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F147" t="s">
+        <v>62</v>
+      </c>
+      <c r="G147" t="s">
         <v>63</v>
       </c>
-      <c r="G147" t="s">
+      <c r="H147" t="s">
         <v>64</v>
       </c>
-      <c r="H147" t="s">
-        <v>65</v>
-      </c>
       <c r="I147" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B151" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C151" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="152" spans="1:11" x14ac:dyDescent="0.25">
@@ -3892,59 +3956,59 @@
         <v>42972</v>
       </c>
       <c r="B152" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C152" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D152" s="10">
         <v>0.3125</v>
       </c>
       <c r="E152" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F152" t="s">
+        <v>62</v>
+      </c>
+      <c r="G152" t="s">
         <v>63</v>
       </c>
-      <c r="G152" t="s">
+      <c r="H152" t="s">
         <v>64</v>
       </c>
-      <c r="H152" t="s">
-        <v>65</v>
-      </c>
       <c r="I152" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B156" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C156" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C158" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D158" s="11">
         <v>8.4124999999999996</v>

</xml_diff>